<commit_message>
always update col Total whether any data or not
</commit_message>
<xml_diff>
--- a/AttendanceChecking.xlsx
+++ b/AttendanceChecking.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8190" windowWidth="16380" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="144525" fullCalcOnLoad="1" iterateDelta="0.0001"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="133">
   <si>
     <t>DANH SÁCH SINH VIÊN</t>
   </si>
@@ -25,7 +25,7 @@
     <t>1 = present</t>
   </si>
   <si>
-    <t>0 = absent</t>
+    <t>blank = absent</t>
   </si>
   <si>
     <t>ID</t>
@@ -418,68 +418,72 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
-      <family val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="13"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
-      <family val="1"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="13"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="13"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="13"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="13"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <b val="1"/>
-      <strike val="0"/>
-      <color rgb="00000000"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -531,53 +535,83 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -867,1408 +901,1415 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALY74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="10.25"/>
-    <col customWidth="1" max="2" min="2" style="11" width="21.875"/>
-    <col customWidth="1" max="3" min="3" style="11" width="15.25"/>
-    <col customWidth="1" max="4" min="4" style="11" width="12.875"/>
-    <col customWidth="1" max="1013" min="5" style="11" width="9.125"/>
-    <col customWidth="1" max="1017" min="1014" style="1" width="11.5"/>
+    <col min="1" max="1" width="10.25" style="10" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.25" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="1009" width="9.125" style="10" customWidth="1"/>
+    <col min="1010" max="1013" width="11.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="16.15" r="1" s="1" spans="1:13">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="2" s="1" spans="1:13">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="3" s="1" spans="1:13">
-      <c r="A3" s="4" t="n"/>
-      <c r="B3" s="4" t="n"/>
-      <c r="C3" s="4" t="n"/>
-      <c r="D3" s="5" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="16.15" r="4" s="1" spans="1:13">
-      <c r="A4" s="4" t="n"/>
-      <c r="B4" s="4" t="n"/>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="5" t="s">
+    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="16.15" r="5" s="2" spans="1:13">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row customHeight="1" ht="16.15" r="6" s="1" spans="1:13">
-      <c r="A6" s="8" t="n">
+    <row r="6" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>1511844</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="n"/>
+      <c r="E6" s="6"/>
       <c r="L6">
-        <f>COUNTBLANK(E6:H6)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="7" s="1" spans="1:13">
-      <c r="A7" s="9" t="n">
+        <f>COUNTBLANK(E6:K6)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>1512221</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="8">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="n"/>
+      <c r="E7" s="6"/>
       <c r="L7">
-        <f>COUNTBLANK(E7:H7)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="8" s="1" spans="1:13">
-      <c r="A8" s="9" t="n">
+        <f>COUNTBLANK(E7:K7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <v>1512396</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="E8" s="7" t="n"/>
+      <c r="E8" s="6"/>
       <c r="L8">
-        <f>COUNTBLANK(E8:H8)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="9" s="1" spans="1:13">
-      <c r="A9" s="9" t="n">
+        <f>COUNTBLANK(E8:K8)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <v>1512534</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="8">
         <v>1</v>
       </c>
-      <c r="E9" s="7" t="n"/>
+      <c r="E9" s="6"/>
       <c r="L9">
-        <f>COUNTBLANK(E9:H9)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="10" s="1" spans="1:13">
-      <c r="A10" s="9" t="n">
+        <f>COUNTBLANK(E9:K9)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>1512640</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="8">
         <v>1</v>
       </c>
-      <c r="E10" s="7" t="n"/>
+      <c r="E10" s="6"/>
       <c r="L10">
-        <f>COUNTBLANK(E10:H10)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="11" s="1" spans="1:13">
-      <c r="A11" s="9" t="n">
+        <f>COUNTBLANK(E10:K10)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <v>1510335</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="9" t="n">
+      <c r="D11" s="8">
         <v>2</v>
       </c>
-      <c r="E11" s="7" t="n"/>
+      <c r="E11" s="6"/>
       <c r="L11">
-        <f>COUNTBLANK(E11:H11)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="12" s="1" spans="1:13">
-      <c r="A12" s="9" t="n">
+        <f>COUNTBLANK(E11:K11)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
         <v>1511234</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="9" t="n">
+      <c r="D12" s="8">
         <v>2</v>
       </c>
-      <c r="E12" s="7" t="n"/>
+      <c r="E12" s="6"/>
       <c r="L12">
-        <f>COUNTBLANK(E12:H12)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="13" s="1" spans="1:13">
-      <c r="A13" s="9" t="n">
+        <f>COUNTBLANK(E12:K12)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <v>1511908</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="9" t="n">
+      <c r="D13" s="8">
         <v>2</v>
       </c>
-      <c r="E13" s="7" t="n"/>
+      <c r="E13" s="6"/>
       <c r="L13">
-        <f>COUNTBLANK(E13:H13)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="14" s="1" spans="1:13">
-      <c r="A14" s="9" t="n">
+        <f>COUNTBLANK(E13:K13)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>1513218</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="9" t="n">
+      <c r="D14" s="8">
         <v>2</v>
       </c>
-      <c r="E14" s="7" t="n"/>
+      <c r="E14" s="6"/>
       <c r="L14">
-        <f>COUNTBLANK(E14:H14)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="15" s="1" spans="1:13">
-      <c r="A15" s="9" t="n">
+        <f>COUNTBLANK(E14:K14)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
         <v>1510806</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="9" t="n">
+      <c r="D15" s="8">
         <v>2</v>
       </c>
-      <c r="E15" s="7" t="n"/>
+      <c r="E15" s="6"/>
       <c r="L15">
-        <f>COUNTBLANK(E15:H15)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="16" s="1" spans="1:13">
-      <c r="A16" s="9" t="n">
+        <f>COUNTBLANK(E15:K15)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
         <v>1510126</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="9" t="n">
+      <c r="D16" s="8">
         <v>3</v>
       </c>
-      <c r="E16" s="7" t="n"/>
+      <c r="E16" s="6"/>
       <c r="L16">
-        <f>COUNTBLANK(E16:H16)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="17" s="1" spans="1:13">
-      <c r="A17" s="9" t="n">
+        <f>COUNTBLANK(E16:K16)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
         <v>1510462</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="9" t="n">
+      <c r="D17" s="8">
         <v>3</v>
       </c>
-      <c r="E17" s="7" t="n"/>
+      <c r="E17" s="6"/>
       <c r="L17">
-        <f>COUNTBLANK(E17:H17)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="18" s="1" spans="1:13">
-      <c r="A18" s="9" t="n">
+        <f>COUNTBLANK(E17:K17)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
         <v>1511766</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="9" t="n">
+      <c r="D18" s="8">
         <v>3</v>
       </c>
-      <c r="E18" s="7" t="n"/>
+      <c r="E18" s="6"/>
       <c r="L18">
-        <f>COUNTBLANK(E18:H18)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="19" s="1" spans="1:13">
-      <c r="A19" s="9" t="n">
+        <f>COUNTBLANK(E18:K18)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
         <v>1512676</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="9" t="n">
+      <c r="D19" s="8">
         <v>3</v>
       </c>
-      <c r="E19" s="7" t="n"/>
+      <c r="E19" s="6"/>
       <c r="L19">
-        <f>COUNTBLANK(E19:H19)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="20" s="1" spans="1:13">
-      <c r="A20" s="9" t="n">
+        <f>COUNTBLANK(E19:K19)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
         <v>1510827</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="9" t="n">
+      <c r="D20" s="8">
         <v>3</v>
       </c>
-      <c r="E20" s="7" t="n"/>
+      <c r="E20" s="6"/>
       <c r="L20">
-        <f>COUNTBLANK(E20:H20)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="21" s="1" spans="1:13">
-      <c r="A21" s="9" t="n">
+        <f>COUNTBLANK(E20:K20)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
         <v>1510463</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="9" t="n">
+      <c r="D21" s="8">
         <v>4</v>
       </c>
-      <c r="E21" s="7" t="n"/>
+      <c r="E21" s="6"/>
       <c r="L21">
-        <f>COUNTBLANK(E21:H21)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="22" s="1" spans="1:13">
-      <c r="A22" s="9" t="n">
+        <f>COUNTBLANK(E21:K21)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
         <v>1513031</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="8">
         <v>4</v>
       </c>
-      <c r="E22" s="7" t="n"/>
+      <c r="E22" s="6"/>
       <c r="L22">
-        <f>COUNTBLANK(E22:H22)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="23" s="1" spans="1:13">
-      <c r="A23" s="9" t="n">
+        <f>COUNTBLANK(E22:K22)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
         <v>1514125</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="8">
         <v>4</v>
       </c>
-      <c r="E23" s="7" t="n"/>
+      <c r="E23" s="6"/>
       <c r="L23">
-        <f>COUNTBLANK(E23:H23)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="24" s="1" spans="1:13">
-      <c r="A24" s="9" t="n">
+        <f>COUNTBLANK(E23:K23)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
         <v>1510652</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="9" t="n">
+      <c r="D24" s="8">
         <v>4</v>
       </c>
-      <c r="E24" s="7" t="n"/>
+      <c r="E24" s="6"/>
       <c r="L24">
-        <f>COUNTBLANK(E24:H24)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="25" s="1" spans="1:13">
-      <c r="A25" s="9" t="n">
+        <f>COUNTBLANK(E24:K24)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
         <v>1510698</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="9" t="n">
+      <c r="D25" s="8">
         <v>4</v>
       </c>
-      <c r="E25" s="7" t="n"/>
+      <c r="E25" s="6"/>
       <c r="L25">
-        <f>COUNTBLANK(E25:H25)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="26" s="1" spans="1:13">
-      <c r="A26" s="9" t="n">
+        <f>COUNTBLANK(E25:K25)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
         <v>1510122</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="9" t="n">
+      <c r="D26" s="8">
         <v>5</v>
       </c>
-      <c r="E26" s="7" t="n"/>
+      <c r="E26" s="6"/>
       <c r="L26">
-        <f>COUNTBLANK(E26:H26)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="27" s="1" spans="1:13">
-      <c r="A27" s="9" t="n">
+        <f>COUNTBLANK(E26:K26)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
         <v>1511021</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="9" t="n">
+      <c r="D27" s="8">
         <v>5</v>
       </c>
-      <c r="E27" s="7" t="n"/>
+      <c r="E27" s="6"/>
       <c r="L27">
-        <f>COUNTBLANK(E27:H27)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="28" s="1" spans="1:13">
-      <c r="A28" s="9" t="n">
+        <f>COUNTBLANK(E27:K27)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
         <v>1511149</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="9" t="n">
+      <c r="D28" s="8">
         <v>5</v>
       </c>
-      <c r="E28" s="7" t="n"/>
+      <c r="E28" s="6"/>
       <c r="L28">
-        <f>COUNTBLANK(E28:H28)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="29" s="1" spans="1:13">
-      <c r="A29" s="9" t="n">
+        <f>COUNTBLANK(E28:K28)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
         <v>1512263</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="9" t="n">
+      <c r="D29" s="8">
         <v>5</v>
       </c>
-      <c r="E29" s="7" t="n"/>
+      <c r="E29" s="6"/>
       <c r="L29">
-        <f>COUNTBLANK(E29:H29)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="30" s="1" spans="1:13">
-      <c r="A30" s="9" t="n">
+        <f>COUNTBLANK(E29:K29)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
         <v>1513524</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="9" t="n">
+      <c r="D30" s="8">
         <v>5</v>
       </c>
-      <c r="E30" s="7" t="n"/>
+      <c r="E30" s="6"/>
       <c r="L30">
-        <f>COUNTBLANK(E30:H30)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="31" s="1" spans="1:13">
-      <c r="A31" s="9" t="n">
+        <f>COUNTBLANK(E30:K30)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
         <v>1512705</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="9" t="n">
+      <c r="D31" s="8">
         <v>6</v>
       </c>
-      <c r="E31" s="7" t="n"/>
+      <c r="E31" s="6"/>
       <c r="L31">
-        <f>COUNTBLANK(E31:H31)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="25.35" r="32" s="1" spans="1:13">
-      <c r="A32" s="9" t="n">
+        <f>COUNTBLANK(E31:K31)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
         <v>1513489</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="9" t="n">
+      <c r="D32" s="8">
         <v>6</v>
       </c>
-      <c r="E32" s="7" t="n"/>
+      <c r="E32" s="6"/>
       <c r="L32">
-        <f>COUNTBLANK(E32:H32)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="33" s="1" spans="1:13">
-      <c r="A33" s="9" t="n">
+        <f>COUNTBLANK(E32:K32)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
         <v>1513505</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="9" t="n">
+      <c r="D33" s="8">
         <v>6</v>
       </c>
-      <c r="E33" s="7" t="n"/>
+      <c r="E33" s="6"/>
       <c r="L33">
-        <f>COUNTBLANK(E33:H33)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="34" s="1" spans="1:13">
-      <c r="A34" s="9" t="n">
+        <f>COUNTBLANK(E33:K33)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
         <v>1533720</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="9" t="n">
+      <c r="D34" s="8">
         <v>6</v>
       </c>
-      <c r="E34" s="7" t="n"/>
+      <c r="E34" s="6"/>
       <c r="L34">
-        <f>COUNTBLANK(E34:H34)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="35" s="1" spans="1:13">
-      <c r="A35" s="9" t="n">
+        <f>COUNTBLANK(E34:K34)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
         <v>1410285</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E35" s="7" t="n"/>
+      <c r="D35" s="8">
+        <v>7</v>
+      </c>
+      <c r="E35" s="6"/>
       <c r="L35">
-        <f>COUNTBLANK(E35:H35)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="36" s="1" spans="1:13">
-      <c r="A36" s="9" t="n">
+        <f>COUNTBLANK(E35:K35)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
         <v>1410397</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E36" s="7" t="n"/>
+      <c r="D36" s="8">
+        <v>7</v>
+      </c>
+      <c r="E36" s="6"/>
       <c r="L36">
-        <f>COUNTBLANK(E36:H36)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="37" s="1" spans="1:13">
-      <c r="A37" s="9" t="n">
+        <f>COUNTBLANK(E36:K36)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
         <v>1412103</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E37" s="7" t="n"/>
+      <c r="D37" s="8">
+        <v>7</v>
+      </c>
+      <c r="E37" s="6"/>
       <c r="L37">
-        <f>COUNTBLANK(E37:H37)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="38" s="1" spans="1:13">
-      <c r="A38" s="9" t="n">
+        <f>COUNTBLANK(E37:K37)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
         <v>1512510</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E38" s="7" t="n"/>
+      <c r="D38" s="8">
+        <v>7</v>
+      </c>
+      <c r="E38" s="6"/>
       <c r="L38">
-        <f>COUNTBLANK(E38:H38)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="39" s="1" spans="1:13">
-      <c r="A39" s="9" t="n">
+        <f>COUNTBLANK(E38:K38)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
         <v>1413471</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E39" s="7" t="n"/>
+      <c r="D39" s="8">
+        <v>7</v>
+      </c>
+      <c r="E39" s="6"/>
       <c r="L39">
-        <f>COUNTBLANK(E39:H39)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="40" s="1" spans="1:13">
-      <c r="A40" s="9" t="n">
+        <f>COUNTBLANK(E39:K39)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
         <v>1510322</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="9" t="n">
+      <c r="D40" s="8">
         <v>8</v>
       </c>
-      <c r="E40" s="7" t="n"/>
+      <c r="E40" s="6"/>
       <c r="L40">
-        <f>COUNTBLANK(E40:H40)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="41" s="1" spans="1:13">
-      <c r="A41" s="9" t="n">
+        <f>COUNTBLANK(E40:K40)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
         <v>1512022</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="9" t="n">
+      <c r="D41" s="8">
         <v>8</v>
       </c>
-      <c r="E41" s="7" t="n"/>
+      <c r="E41" s="6"/>
       <c r="L41">
-        <f>COUNTBLANK(E41:H41)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="42" s="1" spans="1:13">
-      <c r="A42" s="9" t="n">
+        <f>COUNTBLANK(E41:K41)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
         <v>1512830</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="9" t="n">
+      <c r="D42" s="8">
         <v>8</v>
       </c>
-      <c r="E42" s="7" t="n"/>
+      <c r="E42" s="6"/>
       <c r="L42">
-        <f>COUNTBLANK(E42:H42)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="43" s="1" spans="1:13">
-      <c r="A43" s="9" t="n">
+        <f>COUNTBLANK(E42:K42)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
         <v>1513555</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="9" t="n">
+      <c r="D43" s="8">
         <v>8</v>
       </c>
-      <c r="E43" s="7" t="n"/>
+      <c r="E43" s="6"/>
       <c r="L43">
-        <f>COUNTBLANK(E43:H43)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="44" s="1" spans="1:13">
-      <c r="A44" s="9" t="n">
+        <f>COUNTBLANK(E43:K43)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
         <v>1513776</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="9" t="n">
+      <c r="D44" s="8">
         <v>8</v>
       </c>
-      <c r="E44" s="7" t="n"/>
+      <c r="E44" s="6"/>
       <c r="L44">
-        <f>COUNTBLANK(E44:H44)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="45" s="1" spans="1:13">
-      <c r="A45" s="9" t="n">
+        <f>COUNTBLANK(E44:K44)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="8">
         <v>1512489</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D45" s="9" t="n">
+      <c r="D45" s="8">
         <v>9</v>
       </c>
-      <c r="E45" s="7" t="n"/>
+      <c r="E45" s="6"/>
       <c r="L45">
-        <f>COUNTBLANK(E45:H45)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="46" s="1" spans="1:13">
-      <c r="A46" s="9" t="n">
+        <f>COUNTBLANK(E45:K45)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
         <v>1512579</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D46" s="9" t="n">
+      <c r="D46" s="8">
         <v>9</v>
       </c>
-      <c r="E46" s="7" t="n">
+      <c r="E46" s="6">
         <v>1</v>
       </c>
       <c r="L46">
-        <f>COUNTBLANK(E46:H46)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="47" s="1" spans="1:13">
-      <c r="A47" s="9" t="n">
+        <f>COUNTBLANK(E46:K46)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8">
         <v>1512702</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="9" t="n">
+      <c r="D47" s="8">
         <v>9</v>
       </c>
-      <c r="E47" s="7" t="n"/>
+      <c r="E47" s="6"/>
       <c r="L47">
-        <f>COUNTBLANK(E47:H47)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="48" s="1" spans="1:13">
-      <c r="A48" s="9" t="n">
+        <f>COUNTBLANK(E47:K47)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="8">
         <v>1512872</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="9" t="n">
+      <c r="D48" s="8">
         <v>9</v>
       </c>
-      <c r="E48" s="7" t="n"/>
-      <c r="F48" t="n">
+      <c r="E48" s="6"/>
+      <c r="F48">
         <v>1</v>
       </c>
-      <c r="G48" t="n">
+      <c r="G48">
         <v>1</v>
       </c>
-      <c r="H48" t="n">
+      <c r="H48">
         <v>1</v>
       </c>
       <c r="L48">
-        <f>COUNTBLANK(E48:H48)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="49" s="1" spans="1:13">
-      <c r="A49" s="9" t="n">
+        <f>COUNTBLANK(E48:K48)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="8">
         <v>1513172</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="9" t="n">
+      <c r="D49" s="8">
         <v>9</v>
       </c>
-      <c r="E49" s="7" t="n"/>
+      <c r="E49" s="6"/>
       <c r="L49">
-        <f>COUNTBLANK(E49:H49)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="50" s="1" spans="1:13">
-      <c r="A50" s="9" t="n">
+        <f>COUNTBLANK(E49:K49)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8">
         <v>1513372</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="9" t="n">
+      <c r="D50" s="8">
         <v>9</v>
       </c>
-      <c r="E50" s="7" t="n">
+      <c r="E50" s="6">
         <v>1</v>
       </c>
       <c r="L50">
-        <f>COUNTBLANK(E50:H50)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="51" s="1" spans="1:13">
-      <c r="A51" s="9" t="n">
+        <f>COUNTBLANK(E50:K50)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="8">
         <v>1510042</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="9" t="n">
+      <c r="D51" s="8">
         <v>10</v>
       </c>
-      <c r="E51" s="7" t="n"/>
+      <c r="E51" s="6"/>
       <c r="L51">
-        <f>COUNTBLANK(E51:H51)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="52" s="1" spans="1:13">
-      <c r="A52" s="9" t="n">
+        <f>COUNTBLANK(E51:K51)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="8">
         <v>1510391</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D52" s="9" t="n">
+      <c r="D52" s="8">
         <v>10</v>
       </c>
-      <c r="E52" s="7" t="n"/>
+      <c r="E52" s="6"/>
       <c r="L52">
-        <f>COUNTBLANK(E52:H52)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="53" s="1" spans="1:13">
-      <c r="A53" s="9" t="n">
+        <f>COUNTBLANK(E52:K52)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8">
         <v>1511734</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D53" s="9" t="n">
+      <c r="D53" s="8">
         <v>10</v>
       </c>
-      <c r="E53" s="7" t="n"/>
+      <c r="E53" s="6"/>
       <c r="L53">
-        <f>COUNTBLANK(E53:H53)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="54" s="1" spans="1:13">
-      <c r="A54" s="9" t="n">
+        <f>COUNTBLANK(E53:K53)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8">
         <v>1513058</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D54" s="9" t="n">
+      <c r="D54" s="8">
         <v>10</v>
       </c>
-      <c r="E54" s="7" t="n"/>
+      <c r="E54" s="6"/>
       <c r="L54">
-        <f>COUNTBLANK(E54:H54)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="55" s="1" spans="1:13">
-      <c r="A55" s="9" t="n">
+        <f>COUNTBLANK(E54:K54)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8">
         <v>1510484</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="9" t="n">
+      <c r="D55" s="8">
         <v>11</v>
       </c>
-      <c r="E55" s="7" t="n"/>
+      <c r="E55" s="6"/>
       <c r="L55">
-        <f>COUNTBLANK(E55:H55)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="56" s="1" spans="1:13">
-      <c r="A56" s="9" t="n">
+        <f>COUNTBLANK(E55:K55)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="8">
         <v>1511025</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="9" t="n">
+      <c r="D56" s="8">
         <v>11</v>
       </c>
-      <c r="E56" s="7" t="n"/>
+      <c r="E56" s="6"/>
       <c r="L56">
-        <f>COUNTBLANK(E56:H56)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="57" s="1" spans="1:13">
-      <c r="A57" s="9" t="n">
+        <f>COUNTBLANK(E56:K56)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="8">
         <v>1511979</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D57" s="9" t="n">
+      <c r="D57" s="8">
         <v>11</v>
       </c>
-      <c r="E57" s="7" t="n"/>
+      <c r="E57" s="6"/>
       <c r="L57">
-        <f>COUNTBLANK(E57:H57)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="58" s="1" spans="1:13">
-      <c r="A58" s="9" t="n">
+        <f>COUNTBLANK(E57:K57)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="8">
         <v>1512217</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D58" s="9" t="n">
+      <c r="D58" s="8">
         <v>11</v>
       </c>
-      <c r="E58" s="7" t="n"/>
+      <c r="E58" s="6"/>
       <c r="L58">
-        <f>COUNTBLANK(E58:H58)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="59" s="1" spans="1:13">
-      <c r="A59" s="9" t="n">
+        <f>COUNTBLANK(E58:K58)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="8">
         <v>1513614</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="9" t="n">
+      <c r="D59" s="8">
         <v>11</v>
       </c>
-      <c r="E59" s="7" t="n"/>
+      <c r="E59" s="6"/>
       <c r="L59">
-        <f>COUNTBLANK(E59:H59)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="60" s="1" spans="1:13">
-      <c r="A60" s="9" t="n">
+        <f>COUNTBLANK(E59:K59)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="8">
         <v>1410178</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D60" s="9" t="n">
+      <c r="D60" s="8">
         <v>12</v>
       </c>
-      <c r="E60" s="7" t="n"/>
+      <c r="E60" s="6"/>
       <c r="L60">
-        <f>COUNTBLANK(E60:H60)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="61" s="1" spans="1:13">
-      <c r="A61" s="9" t="n">
+        <f>COUNTBLANK(E60:K60)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="8">
         <v>1510274</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D61" s="9" t="n">
+      <c r="D61" s="8">
         <v>12</v>
       </c>
-      <c r="E61" s="7" t="n"/>
+      <c r="E61" s="6"/>
       <c r="L61">
-        <f>COUNTBLANK(E61:H61)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="62" s="1" spans="1:13">
-      <c r="A62" s="9" t="n">
+        <f>COUNTBLANK(E61:K61)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="8">
         <v>1511440</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D62" s="9" t="n">
+      <c r="D62" s="8">
         <v>12</v>
       </c>
-      <c r="E62" s="7" t="n"/>
+      <c r="E62" s="6"/>
       <c r="L62">
-        <f>COUNTBLANK(E62:H62)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="63" s="1" spans="1:13">
-      <c r="A63" s="9" t="n">
+        <f>COUNTBLANK(E62:K62)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="8">
         <v>1411801</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D63" s="9" t="n">
+      <c r="D63" s="8">
         <v>12</v>
       </c>
-      <c r="E63" s="7" t="n"/>
+      <c r="E63" s="6"/>
       <c r="L63">
-        <f>COUNTBLANK(E63:H63)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="64" s="1" spans="1:13">
-      <c r="A64" s="9" t="n">
+        <f>COUNTBLANK(E63:K63)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="8">
         <v>1610811</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D64" s="9" t="n">
+      <c r="D64" s="8">
         <v>13</v>
       </c>
-      <c r="E64" s="7" t="n"/>
+      <c r="E64" s="6"/>
       <c r="L64">
-        <f>COUNTBLANK(E64:H64)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="65" s="1" spans="1:13">
-      <c r="A65" s="9" t="n">
+        <f>COUNTBLANK(E64:K64)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="8">
         <v>1620052</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D65" s="9" t="n">
+      <c r="D65" s="8">
         <v>13</v>
       </c>
-      <c r="E65" s="7" t="n"/>
+      <c r="E65" s="6"/>
       <c r="L65">
-        <f>COUNTBLANK(E65:H65)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="66" s="1" spans="1:13">
-      <c r="A66" s="9" t="n">
+        <f>COUNTBLANK(E65:K65)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="8">
         <v>1513467</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D66" s="9" t="n">
+      <c r="D66" s="8">
         <v>13</v>
       </c>
-      <c r="E66" s="7" t="n"/>
+      <c r="E66" s="6"/>
       <c r="L66">
-        <f>COUNTBLANK(E66:H66)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="67" s="1" spans="1:13">
-      <c r="A67" s="9" t="n">
+        <f>COUNTBLANK(E66:K66)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="8">
         <v>1510332</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D67" s="9" t="n">
+      <c r="D67" s="8">
         <v>14</v>
       </c>
-      <c r="E67" s="7" t="n"/>
+      <c r="E67" s="6"/>
       <c r="L67">
-        <f>COUNTBLANK(E67:H67)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="68" s="1" spans="1:13">
-      <c r="A68" s="9" t="n">
+        <f>COUNTBLANK(E67:K67)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="8">
         <v>1510830</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D68" s="9" t="n">
+      <c r="D68" s="8">
         <v>14</v>
       </c>
-      <c r="E68" s="7" t="n"/>
+      <c r="E68" s="6"/>
       <c r="L68">
-        <f>COUNTBLANK(E68:H68)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="69" s="1" spans="1:13">
-      <c r="A69" s="9" t="n">
+        <f>COUNTBLANK(E68:K68)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="8">
         <v>1512296</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D69" s="9" t="n">
+      <c r="D69" s="8">
         <v>14</v>
       </c>
-      <c r="E69" s="7" t="n"/>
+      <c r="E69" s="6"/>
       <c r="L69">
-        <f>COUNTBLANK(E69:H69)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="70" s="1" spans="1:13">
-      <c r="A70" s="9" t="n">
+        <f>COUNTBLANK(E69:K69)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="8">
         <v>1512312</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D70" s="9" t="n">
+      <c r="D70" s="8">
         <v>14</v>
       </c>
-      <c r="E70" s="7" t="n"/>
-      <c r="L70" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="71" s="1" spans="1:13">
-      <c r="A71" s="9" t="n">
+      <c r="E70" s="6"/>
+      <c r="L70" s="1">
+        <f>COUNTBLANK(E70:K70)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8">
         <v>1511013</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="9" t="n">
+      <c r="D71" s="8">
         <v>15</v>
       </c>
-      <c r="E71" s="7" t="n"/>
-      <c r="L71" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="72" s="1" spans="1:13">
-      <c r="A72" s="9" t="n">
+      <c r="E71" s="6"/>
+      <c r="L71" s="1">
+        <f>COUNTBLANK(E71:K71)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="8">
         <v>1511552</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D72" s="9" t="n">
+      <c r="D72" s="8">
         <v>15</v>
       </c>
-      <c r="E72" s="7" t="n"/>
-      <c r="L72" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="73" s="1" spans="1:13">
-      <c r="A73" s="9" t="n">
+      <c r="E72" s="6"/>
+      <c r="L72" s="1">
+        <f>COUNTBLANK(E72:K72)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="8">
         <v>1513157</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D73" s="9" t="n">
+      <c r="D73" s="8">
         <v>15</v>
       </c>
-      <c r="E73" s="7" t="n"/>
-      <c r="L73" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="16.15" r="74" s="1" spans="1:13">
-      <c r="A74" s="9" t="n">
+      <c r="E73" s="6"/>
+      <c r="L73" s="1">
+        <f>COUNTBLANK(E73:K73)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="8">
         <v>1410947</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D74" s="9" t="n">
+      <c r="D74" s="8">
         <v>15</v>
       </c>
-      <c r="E74" s="7" t="n"/>
-      <c r="L74" t="n">
-        <v>1</v>
+      <c r="E74" s="6"/>
+      <c r="L74" s="1">
+        <f>COUNTBLANK(E74:K74)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2317,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup firstPageNumber="0" fitToHeight="1" fitToWidth="10" horizontalDpi="300" orientation="landscape" paperSize="9" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToWidth="10" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix error when using wrong excel file and add wrong file
</commit_message>
<xml_diff>
--- a/AttendanceChecking.xlsx
+++ b/AttendanceChecking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="136">
   <si>
     <t>DANH SÁCH SINH VIÊN</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>10/14/2018</t>
+  </si>
+  <si>
+    <t>10/15/2018</t>
   </si>
   <si>
     <t>Total</t>
@@ -963,23 +966,27 @@
       <c r="N5" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="O5" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row customHeight="1" ht="16.15" r="6" s="1" spans="1:15">
       <c r="A6" s="8" t="n">
         <v>1511844</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="n"/>
-      <c r="N6">
-        <f>COUNTBLANK(E6:H6)</f>
+      <c r="N6" t="s"/>
+      <c r="O6">
+        <f>COUNTBLANK(E6:N6)</f>
         <v/>
       </c>
     </row>
@@ -988,17 +995,18 @@
         <v>1512221</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="7" t="n"/>
-      <c r="N7">
-        <f>COUNTBLANK(E7:H7)</f>
+      <c r="N7" t="s"/>
+      <c r="O7">
+        <f>COUNTBLANK(E7:N7)</f>
         <v/>
       </c>
     </row>
@@ -1007,17 +1015,18 @@
         <v>1512396</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="7" t="n"/>
-      <c r="N8">
-        <f>COUNTBLANK(E8:H8)</f>
+      <c r="N8" t="s"/>
+      <c r="O8">
+        <f>COUNTBLANK(E8:N8)</f>
         <v/>
       </c>
     </row>
@@ -1026,17 +1035,18 @@
         <v>1512534</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="n"/>
-      <c r="N9">
-        <f>COUNTBLANK(E9:H9)</f>
+      <c r="N9" t="s"/>
+      <c r="O9">
+        <f>COUNTBLANK(E9:N9)</f>
         <v/>
       </c>
     </row>
@@ -1045,17 +1055,18 @@
         <v>1512640</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="7" t="n"/>
-      <c r="N10">
-        <f>COUNTBLANK(E10:H10)</f>
+      <c r="N10" t="s"/>
+      <c r="O10">
+        <f>COUNTBLANK(E10:N10)</f>
         <v/>
       </c>
     </row>
@@ -1064,17 +1075,18 @@
         <v>1510335</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="9" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="7" t="n"/>
-      <c r="N11">
-        <f>COUNTBLANK(E11:H11)</f>
+      <c r="N11" t="s"/>
+      <c r="O11">
+        <f>COUNTBLANK(E11:N11)</f>
         <v/>
       </c>
     </row>
@@ -1083,17 +1095,18 @@
         <v>1511234</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="9" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="7" t="n"/>
-      <c r="N12">
-        <f>COUNTBLANK(E12:H12)</f>
+      <c r="N12" t="s"/>
+      <c r="O12">
+        <f>COUNTBLANK(E12:N12)</f>
         <v/>
       </c>
     </row>
@@ -1102,17 +1115,18 @@
         <v>1511908</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="9" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="7" t="n"/>
-      <c r="N13">
-        <f>COUNTBLANK(E13:H13)</f>
+      <c r="N13" t="s"/>
+      <c r="O13">
+        <f>COUNTBLANK(E13:N13)</f>
         <v/>
       </c>
     </row>
@@ -1121,17 +1135,18 @@
         <v>1513218</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="9" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="7" t="n"/>
-      <c r="N14">
-        <f>COUNTBLANK(E14:H14)</f>
+      <c r="N14" t="s"/>
+      <c r="O14">
+        <f>COUNTBLANK(E14:N14)</f>
         <v/>
       </c>
     </row>
@@ -1140,17 +1155,18 @@
         <v>1510806</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="9" t="n">
         <v>2</v>
       </c>
       <c r="E15" s="7" t="n"/>
-      <c r="N15">
-        <f>COUNTBLANK(E15:H15)</f>
+      <c r="N15" t="s"/>
+      <c r="O15">
+        <f>COUNTBLANK(E15:N15)</f>
         <v/>
       </c>
     </row>
@@ -1159,17 +1175,18 @@
         <v>1510126</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="9" t="n">
         <v>3</v>
       </c>
       <c r="E16" s="7" t="n"/>
-      <c r="N16">
-        <f>COUNTBLANK(E16:H16)</f>
+      <c r="N16" t="s"/>
+      <c r="O16">
+        <f>COUNTBLANK(E16:N16)</f>
         <v/>
       </c>
     </row>
@@ -1178,17 +1195,18 @@
         <v>1510462</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" s="9" t="n">
         <v>3</v>
       </c>
       <c r="E17" s="7" t="n"/>
-      <c r="N17">
-        <f>COUNTBLANK(E17:H17)</f>
+      <c r="N17" t="s"/>
+      <c r="O17">
+        <f>COUNTBLANK(E17:N17)</f>
         <v/>
       </c>
     </row>
@@ -1197,17 +1215,18 @@
         <v>1511766</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="9" t="n">
         <v>3</v>
       </c>
       <c r="E18" s="7" t="n"/>
-      <c r="N18">
-        <f>COUNTBLANK(E18:H18)</f>
+      <c r="N18" t="s"/>
+      <c r="O18">
+        <f>COUNTBLANK(E18:N18)</f>
         <v/>
       </c>
     </row>
@@ -1216,17 +1235,18 @@
         <v>1512676</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>3</v>
       </c>
       <c r="E19" s="7" t="n"/>
-      <c r="N19">
-        <f>COUNTBLANK(E19:H19)</f>
+      <c r="N19" t="s"/>
+      <c r="O19">
+        <f>COUNTBLANK(E19:N19)</f>
         <v/>
       </c>
     </row>
@@ -1235,17 +1255,18 @@
         <v>1510827</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20" s="9" t="n">
         <v>3</v>
       </c>
       <c r="E20" s="7" t="n"/>
-      <c r="N20">
-        <f>COUNTBLANK(E20:H20)</f>
+      <c r="N20" t="s"/>
+      <c r="O20">
+        <f>COUNTBLANK(E20:N20)</f>
         <v/>
       </c>
     </row>
@@ -1254,17 +1275,18 @@
         <v>1510463</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="9" t="n">
         <v>4</v>
       </c>
       <c r="E21" s="7" t="n"/>
-      <c r="N21">
-        <f>COUNTBLANK(E21:H21)</f>
+      <c r="N21" t="s"/>
+      <c r="O21">
+        <f>COUNTBLANK(E21:N21)</f>
         <v/>
       </c>
     </row>
@@ -1273,17 +1295,18 @@
         <v>1513031</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="9" t="n">
         <v>4</v>
       </c>
       <c r="E22" s="7" t="n"/>
-      <c r="N22">
-        <f>COUNTBLANK(E22:H22)</f>
+      <c r="N22" t="s"/>
+      <c r="O22">
+        <f>COUNTBLANK(E22:N22)</f>
         <v/>
       </c>
     </row>
@@ -1292,17 +1315,18 @@
         <v>1514125</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" s="9" t="n">
         <v>4</v>
       </c>
       <c r="E23" s="7" t="n"/>
-      <c r="N23">
-        <f>COUNTBLANK(E23:H23)</f>
+      <c r="N23" t="s"/>
+      <c r="O23">
+        <f>COUNTBLANK(E23:N23)</f>
         <v/>
       </c>
     </row>
@@ -1311,17 +1335,18 @@
         <v>1510652</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" s="9" t="n">
         <v>4</v>
       </c>
       <c r="E24" s="7" t="n"/>
-      <c r="N24">
-        <f>COUNTBLANK(E24:H24)</f>
+      <c r="N24" t="s"/>
+      <c r="O24">
+        <f>COUNTBLANK(E24:N24)</f>
         <v/>
       </c>
     </row>
@@ -1330,17 +1355,18 @@
         <v>1510698</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="9" t="n">
         <v>4</v>
       </c>
       <c r="E25" s="7" t="n"/>
-      <c r="N25">
-        <f>COUNTBLANK(E25:H25)</f>
+      <c r="N25" t="s"/>
+      <c r="O25">
+        <f>COUNTBLANK(E25:N25)</f>
         <v/>
       </c>
     </row>
@@ -1349,17 +1375,18 @@
         <v>1510122</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D26" s="9" t="n">
         <v>5</v>
       </c>
       <c r="E26" s="7" t="n"/>
-      <c r="N26">
-        <f>COUNTBLANK(E26:H26)</f>
+      <c r="N26" t="s"/>
+      <c r="O26">
+        <f>COUNTBLANK(E26:N26)</f>
         <v/>
       </c>
     </row>
@@ -1368,17 +1395,18 @@
         <v>1511021</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="9" t="n">
         <v>5</v>
       </c>
       <c r="E27" s="7" t="n"/>
-      <c r="N27">
-        <f>COUNTBLANK(E27:H27)</f>
+      <c r="N27" t="s"/>
+      <c r="O27">
+        <f>COUNTBLANK(E27:N27)</f>
         <v/>
       </c>
     </row>
@@ -1387,17 +1415,18 @@
         <v>1511149</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D28" s="9" t="n">
         <v>5</v>
       </c>
       <c r="E28" s="7" t="n"/>
-      <c r="N28">
-        <f>COUNTBLANK(E28:H28)</f>
+      <c r="N28" t="s"/>
+      <c r="O28">
+        <f>COUNTBLANK(E28:N28)</f>
         <v/>
       </c>
     </row>
@@ -1406,17 +1435,18 @@
         <v>1512263</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D29" s="9" t="n">
         <v>5</v>
       </c>
       <c r="E29" s="7" t="n"/>
-      <c r="N29">
-        <f>COUNTBLANK(E29:H29)</f>
+      <c r="N29" t="s"/>
+      <c r="O29">
+        <f>COUNTBLANK(E29:N29)</f>
         <v/>
       </c>
     </row>
@@ -1425,17 +1455,18 @@
         <v>1513524</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D30" s="9" t="n">
         <v>5</v>
       </c>
       <c r="E30" s="7" t="n"/>
-      <c r="N30">
-        <f>COUNTBLANK(E30:H30)</f>
+      <c r="N30" t="s"/>
+      <c r="O30">
+        <f>COUNTBLANK(E30:N30)</f>
         <v/>
       </c>
     </row>
@@ -1444,17 +1475,18 @@
         <v>1512705</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D31" s="9" t="n">
         <v>6</v>
       </c>
       <c r="E31" s="7" t="n"/>
-      <c r="N31">
-        <f>COUNTBLANK(E31:H31)</f>
+      <c r="N31" t="s"/>
+      <c r="O31">
+        <f>COUNTBLANK(E31:N31)</f>
         <v/>
       </c>
     </row>
@@ -1463,17 +1495,18 @@
         <v>1513489</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D32" s="9" t="n">
         <v>6</v>
       </c>
       <c r="E32" s="7" t="n"/>
-      <c r="N32">
-        <f>COUNTBLANK(E32:H32)</f>
+      <c r="N32" t="s"/>
+      <c r="O32">
+        <f>COUNTBLANK(E32:N32)</f>
         <v/>
       </c>
     </row>
@@ -1482,17 +1515,18 @@
         <v>1513505</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D33" s="9" t="n">
         <v>6</v>
       </c>
       <c r="E33" s="7" t="n"/>
-      <c r="N33">
-        <f>COUNTBLANK(E33:H33)</f>
+      <c r="N33" t="s"/>
+      <c r="O33">
+        <f>COUNTBLANK(E33:N33)</f>
         <v/>
       </c>
     </row>
@@ -1501,17 +1535,18 @@
         <v>1533720</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D34" s="9" t="n">
         <v>6</v>
       </c>
       <c r="E34" s="7" t="n"/>
-      <c r="N34">
-        <f>COUNTBLANK(E34:H34)</f>
+      <c r="N34" t="s"/>
+      <c r="O34">
+        <f>COUNTBLANK(E34:N34)</f>
         <v/>
       </c>
     </row>
@@ -1520,17 +1555,18 @@
         <v>1410285</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D35" s="9" t="n">
         <v>7</v>
       </c>
       <c r="E35" s="7" t="n"/>
-      <c r="N35">
-        <f>COUNTBLANK(E35:H35)</f>
+      <c r="N35" t="s"/>
+      <c r="O35">
+        <f>COUNTBLANK(E35:N35)</f>
         <v/>
       </c>
     </row>
@@ -1539,17 +1575,18 @@
         <v>1410397</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D36" s="9" t="n">
         <v>7</v>
       </c>
       <c r="E36" s="7" t="n"/>
-      <c r="N36">
-        <f>COUNTBLANK(E36:H36)</f>
+      <c r="N36" t="s"/>
+      <c r="O36">
+        <f>COUNTBLANK(E36:N36)</f>
         <v/>
       </c>
     </row>
@@ -1558,17 +1595,18 @@
         <v>1412103</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D37" s="9" t="n">
         <v>7</v>
       </c>
       <c r="E37" s="7" t="n"/>
-      <c r="N37">
-        <f>COUNTBLANK(E37:H37)</f>
+      <c r="N37" t="s"/>
+      <c r="O37">
+        <f>COUNTBLANK(E37:N37)</f>
         <v/>
       </c>
     </row>
@@ -1577,17 +1615,18 @@
         <v>1512510</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D38" s="9" t="n">
         <v>7</v>
       </c>
       <c r="E38" s="7" t="n"/>
-      <c r="N38">
-        <f>COUNTBLANK(E38:H38)</f>
+      <c r="N38" t="s"/>
+      <c r="O38">
+        <f>COUNTBLANK(E38:N38)</f>
         <v/>
       </c>
     </row>
@@ -1596,17 +1635,18 @@
         <v>1413471</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D39" s="9" t="n">
         <v>7</v>
       </c>
       <c r="E39" s="7" t="n"/>
-      <c r="N39">
-        <f>COUNTBLANK(E39:H39)</f>
+      <c r="N39" t="s"/>
+      <c r="O39">
+        <f>COUNTBLANK(E39:N39)</f>
         <v/>
       </c>
     </row>
@@ -1615,17 +1655,18 @@
         <v>1510322</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D40" s="9" t="n">
         <v>8</v>
       </c>
       <c r="E40" s="7" t="n"/>
-      <c r="N40">
-        <f>COUNTBLANK(E40:H40)</f>
+      <c r="N40" t="s"/>
+      <c r="O40">
+        <f>COUNTBLANK(E40:N40)</f>
         <v/>
       </c>
     </row>
@@ -1634,17 +1675,18 @@
         <v>1512022</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D41" s="9" t="n">
         <v>8</v>
       </c>
       <c r="E41" s="7" t="n"/>
-      <c r="N41">
-        <f>COUNTBLANK(E41:H41)</f>
+      <c r="N41" t="s"/>
+      <c r="O41">
+        <f>COUNTBLANK(E41:N41)</f>
         <v/>
       </c>
     </row>
@@ -1653,17 +1695,18 @@
         <v>1512830</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D42" s="9" t="n">
         <v>8</v>
       </c>
       <c r="E42" s="7" t="n"/>
-      <c r="N42">
-        <f>COUNTBLANK(E42:H42)</f>
+      <c r="N42" t="s"/>
+      <c r="O42">
+        <f>COUNTBLANK(E42:N42)</f>
         <v/>
       </c>
     </row>
@@ -1672,17 +1715,18 @@
         <v>1513555</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D43" s="9" t="n">
         <v>8</v>
       </c>
       <c r="E43" s="7" t="n"/>
-      <c r="N43">
-        <f>COUNTBLANK(E43:H43)</f>
+      <c r="N43" t="s"/>
+      <c r="O43">
+        <f>COUNTBLANK(E43:N43)</f>
         <v/>
       </c>
     </row>
@@ -1691,17 +1735,18 @@
         <v>1513776</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D44" s="9" t="n">
         <v>8</v>
       </c>
       <c r="E44" s="7" t="n"/>
-      <c r="N44">
-        <f>COUNTBLANK(E44:H44)</f>
+      <c r="N44" t="s"/>
+      <c r="O44">
+        <f>COUNTBLANK(E44:N44)</f>
         <v/>
       </c>
     </row>
@@ -1710,17 +1755,18 @@
         <v>1512489</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D45" s="9" t="n">
         <v>9</v>
       </c>
       <c r="E45" s="7" t="n"/>
-      <c r="N45">
-        <f>COUNTBLANK(E45:H45)</f>
+      <c r="N45" t="s"/>
+      <c r="O45">
+        <f>COUNTBLANK(E45:N45)</f>
         <v/>
       </c>
     </row>
@@ -1729,10 +1775,10 @@
         <v>1512579</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D46" s="9" t="n">
         <v>9</v>
@@ -1740,8 +1786,9 @@
       <c r="E46" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="N46">
-        <f>COUNTBLANK(E46:H46)</f>
+      <c r="N46" t="s"/>
+      <c r="O46">
+        <f>COUNTBLANK(E46:N46)</f>
         <v/>
       </c>
     </row>
@@ -1750,17 +1797,18 @@
         <v>1512702</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D47" s="9" t="n">
         <v>9</v>
       </c>
       <c r="E47" s="7" t="n"/>
-      <c r="N47">
-        <f>COUNTBLANK(E47:H47)</f>
+      <c r="N47" t="s"/>
+      <c r="O47">
+        <f>COUNTBLANK(E47:N47)</f>
         <v/>
       </c>
     </row>
@@ -1769,10 +1817,10 @@
         <v>1512872</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D48" s="9" t="n">
         <v>9</v>
@@ -1787,8 +1835,9 @@
       <c r="H48" t="n">
         <v>1</v>
       </c>
-      <c r="N48">
-        <f>COUNTBLANK(E48:H48)</f>
+      <c r="N48" t="s"/>
+      <c r="O48">
+        <f>COUNTBLANK(E48:N48)</f>
         <v/>
       </c>
     </row>
@@ -1797,17 +1846,18 @@
         <v>1513172</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D49" s="9" t="n">
         <v>9</v>
       </c>
       <c r="E49" s="7" t="n"/>
-      <c r="N49">
-        <f>COUNTBLANK(E49:H49)</f>
+      <c r="N49" t="s"/>
+      <c r="O49">
+        <f>COUNTBLANK(E49:N49)</f>
         <v/>
       </c>
     </row>
@@ -1816,10 +1866,10 @@
         <v>1513372</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D50" s="9" t="n">
         <v>9</v>
@@ -1827,8 +1877,9 @@
       <c r="E50" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="N50">
-        <f>COUNTBLANK(E50:H50)</f>
+      <c r="N50" t="s"/>
+      <c r="O50">
+        <f>COUNTBLANK(E50:N50)</f>
         <v/>
       </c>
     </row>
@@ -1837,17 +1888,18 @@
         <v>1510042</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D51" s="9" t="n">
         <v>10</v>
       </c>
       <c r="E51" s="7" t="n"/>
-      <c r="N51">
-        <f>COUNTBLANK(E51:H51)</f>
+      <c r="N51" t="s"/>
+      <c r="O51">
+        <f>COUNTBLANK(E51:N51)</f>
         <v/>
       </c>
     </row>
@@ -1856,17 +1908,18 @@
         <v>1510391</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D52" s="9" t="n">
         <v>10</v>
       </c>
       <c r="E52" s="7" t="n"/>
-      <c r="N52">
-        <f>COUNTBLANK(E52:H52)</f>
+      <c r="N52" t="s"/>
+      <c r="O52">
+        <f>COUNTBLANK(E52:N52)</f>
         <v/>
       </c>
     </row>
@@ -1875,17 +1928,18 @@
         <v>1511734</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D53" s="9" t="n">
         <v>10</v>
       </c>
       <c r="E53" s="7" t="n"/>
-      <c r="N53">
-        <f>COUNTBLANK(E53:H53)</f>
+      <c r="N53" t="s"/>
+      <c r="O53">
+        <f>COUNTBLANK(E53:N53)</f>
         <v/>
       </c>
     </row>
@@ -1894,17 +1948,18 @@
         <v>1513058</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D54" s="9" t="n">
         <v>10</v>
       </c>
       <c r="E54" s="7" t="n"/>
-      <c r="N54">
-        <f>COUNTBLANK(E54:H54)</f>
+      <c r="N54" t="s"/>
+      <c r="O54">
+        <f>COUNTBLANK(E54:N54)</f>
         <v/>
       </c>
     </row>
@@ -1913,17 +1968,18 @@
         <v>1510484</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D55" s="9" t="n">
         <v>11</v>
       </c>
       <c r="E55" s="7" t="n"/>
-      <c r="N55">
-        <f>COUNTBLANK(E55:H55)</f>
+      <c r="N55" t="s"/>
+      <c r="O55">
+        <f>COUNTBLANK(E55:N55)</f>
         <v/>
       </c>
     </row>
@@ -1932,17 +1988,18 @@
         <v>1511025</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D56" s="9" t="n">
         <v>11</v>
       </c>
       <c r="E56" s="7" t="n"/>
-      <c r="N56">
-        <f>COUNTBLANK(E56:H56)</f>
+      <c r="N56" t="s"/>
+      <c r="O56">
+        <f>COUNTBLANK(E56:N56)</f>
         <v/>
       </c>
     </row>
@@ -1951,17 +2008,18 @@
         <v>1511979</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D57" s="9" t="n">
         <v>11</v>
       </c>
       <c r="E57" s="7" t="n"/>
-      <c r="N57">
-        <f>COUNTBLANK(E57:H57)</f>
+      <c r="N57" t="s"/>
+      <c r="O57">
+        <f>COUNTBLANK(E57:N57)</f>
         <v/>
       </c>
     </row>
@@ -1970,17 +2028,18 @@
         <v>1512217</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D58" s="9" t="n">
         <v>11</v>
       </c>
       <c r="E58" s="7" t="n"/>
-      <c r="N58">
-        <f>COUNTBLANK(E58:H58)</f>
+      <c r="N58" t="s"/>
+      <c r="O58">
+        <f>COUNTBLANK(E58:N58)</f>
         <v/>
       </c>
     </row>
@@ -1989,17 +2048,18 @@
         <v>1513614</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D59" s="9" t="n">
         <v>11</v>
       </c>
       <c r="E59" s="7" t="n"/>
-      <c r="N59">
-        <f>COUNTBLANK(E59:H59)</f>
+      <c r="N59" t="s"/>
+      <c r="O59">
+        <f>COUNTBLANK(E59:N59)</f>
         <v/>
       </c>
     </row>
@@ -2008,17 +2068,18 @@
         <v>1410178</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D60" s="9" t="n">
         <v>12</v>
       </c>
       <c r="E60" s="7" t="n"/>
-      <c r="N60">
-        <f>COUNTBLANK(E60:H60)</f>
+      <c r="N60" t="s"/>
+      <c r="O60">
+        <f>COUNTBLANK(E60:N60)</f>
         <v/>
       </c>
     </row>
@@ -2027,17 +2088,18 @@
         <v>1510274</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D61" s="9" t="n">
         <v>12</v>
       </c>
       <c r="E61" s="7" t="n"/>
-      <c r="N61">
-        <f>COUNTBLANK(E61:H61)</f>
+      <c r="N61" t="s"/>
+      <c r="O61">
+        <f>COUNTBLANK(E61:N61)</f>
         <v/>
       </c>
     </row>
@@ -2046,17 +2108,18 @@
         <v>1511440</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D62" s="9" t="n">
         <v>12</v>
       </c>
       <c r="E62" s="7" t="n"/>
-      <c r="N62">
-        <f>COUNTBLANK(E62:H62)</f>
+      <c r="N62" t="s"/>
+      <c r="O62">
+        <f>COUNTBLANK(E62:N62)</f>
         <v/>
       </c>
     </row>
@@ -2065,17 +2128,18 @@
         <v>1411801</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D63" s="9" t="n">
         <v>12</v>
       </c>
       <c r="E63" s="7" t="n"/>
-      <c r="N63">
-        <f>COUNTBLANK(E63:H63)</f>
+      <c r="N63" t="s"/>
+      <c r="O63">
+        <f>COUNTBLANK(E63:N63)</f>
         <v/>
       </c>
     </row>
@@ -2084,17 +2148,18 @@
         <v>1610811</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D64" s="9" t="n">
         <v>13</v>
       </c>
       <c r="E64" s="7" t="n"/>
-      <c r="N64">
-        <f>COUNTBLANK(E64:H64)</f>
+      <c r="N64" t="s"/>
+      <c r="O64">
+        <f>COUNTBLANK(E64:N64)</f>
         <v/>
       </c>
     </row>
@@ -2103,17 +2168,18 @@
         <v>1620052</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D65" s="9" t="n">
         <v>13</v>
       </c>
       <c r="E65" s="7" t="n"/>
-      <c r="N65">
-        <f>COUNTBLANK(E65:H65)</f>
+      <c r="N65" t="s"/>
+      <c r="O65">
+        <f>COUNTBLANK(E65:N65)</f>
         <v/>
       </c>
     </row>
@@ -2122,17 +2188,18 @@
         <v>1513467</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D66" s="9" t="n">
         <v>13</v>
       </c>
       <c r="E66" s="7" t="n"/>
-      <c r="N66">
-        <f>COUNTBLANK(E66:H66)</f>
+      <c r="N66" t="s"/>
+      <c r="O66">
+        <f>COUNTBLANK(E66:N66)</f>
         <v/>
       </c>
     </row>
@@ -2141,17 +2208,18 @@
         <v>1510332</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D67" s="9" t="n">
         <v>14</v>
       </c>
       <c r="E67" s="7" t="n"/>
-      <c r="N67">
-        <f>COUNTBLANK(E67:H67)</f>
+      <c r="N67" t="s"/>
+      <c r="O67">
+        <f>COUNTBLANK(E67:N67)</f>
         <v/>
       </c>
     </row>
@@ -2160,17 +2228,18 @@
         <v>1510830</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D68" s="9" t="n">
         <v>14</v>
       </c>
       <c r="E68" s="7" t="n"/>
-      <c r="N68">
-        <f>COUNTBLANK(E68:H68)</f>
+      <c r="N68" t="s"/>
+      <c r="O68">
+        <f>COUNTBLANK(E68:N68)</f>
         <v/>
       </c>
     </row>
@@ -2179,17 +2248,18 @@
         <v>1512296</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D69" s="9" t="n">
         <v>14</v>
       </c>
       <c r="E69" s="7" t="n"/>
-      <c r="N69">
-        <f>COUNTBLANK(E69:H69)</f>
+      <c r="N69" t="s"/>
+      <c r="O69">
+        <f>COUNTBLANK(E69:N69)</f>
         <v/>
       </c>
     </row>
@@ -2198,17 +2268,19 @@
         <v>1512312</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D70" s="9" t="n">
         <v>14</v>
       </c>
       <c r="E70" s="7" t="n"/>
-      <c r="N70" t="n">
-        <v>1</v>
+      <c r="N70" t="s"/>
+      <c r="O70">
+        <f>COUNTBLANK(E70:N70)</f>
+        <v/>
       </c>
     </row>
     <row customHeight="1" ht="16.15" r="71" s="1" spans="1:15">
@@ -2216,17 +2288,19 @@
         <v>1511013</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D71" s="9" t="n">
         <v>15</v>
       </c>
       <c r="E71" s="7" t="n"/>
-      <c r="N71" t="n">
-        <v>1</v>
+      <c r="N71" t="s"/>
+      <c r="O71">
+        <f>COUNTBLANK(E71:N71)</f>
+        <v/>
       </c>
     </row>
     <row customHeight="1" ht="16.15" r="72" s="1" spans="1:15">
@@ -2234,17 +2308,19 @@
         <v>1511552</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D72" s="9" t="n">
         <v>15</v>
       </c>
       <c r="E72" s="7" t="n"/>
-      <c r="N72" t="n">
-        <v>1</v>
+      <c r="N72" t="s"/>
+      <c r="O72">
+        <f>COUNTBLANK(E72:N72)</f>
+        <v/>
       </c>
     </row>
     <row customHeight="1" ht="16.15" r="73" s="1" spans="1:15">
@@ -2252,17 +2328,19 @@
         <v>1513157</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D73" s="9" t="n">
         <v>15</v>
       </c>
       <c r="E73" s="7" t="n"/>
-      <c r="N73" t="n">
-        <v>1</v>
+      <c r="N73" t="s"/>
+      <c r="O73">
+        <f>COUNTBLANK(E73:N73)</f>
+        <v/>
       </c>
     </row>
     <row customHeight="1" ht="16.15" r="74" s="1" spans="1:15">
@@ -2270,17 +2348,19 @@
         <v>1410947</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D74" s="9" t="n">
         <v>15</v>
       </c>
       <c r="E74" s="7" t="n"/>
-      <c r="N74" t="n">
-        <v>1</v>
+      <c r="N74" t="s"/>
+      <c r="O74">
+        <f>COUNTBLANK(E74:N74)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>